<commit_message>
Added the Wohlen Data and fitted the model again
</commit_message>
<xml_diff>
--- a/Wetterdaten_Wohlen.xlsx
+++ b/Wetterdaten_Wohlen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ktag365-my.sharepoint.com/personal/jan_siegenthaler_ag_ch/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSIO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003AE89D-AD89-4C72-B418-0C696DE6C3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7974BEDC-F938-4DA3-BF90-12DBD67FE912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4B81F84A-9435-43FD-A46C-35236CA5C320}"/>
   </bookViews>
@@ -411,8 +411,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:F938"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -458,7 +458,7 @@
         <v>50.399999999999991</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>27.114285714285717</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
         <v>5.8999999999999995</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>39.98571428571428</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>23.442857142857143</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>9.1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>19.528571428571432</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>35.800000000000004</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>29.87142857142857</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>28.2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>29.914285714285715</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -584,7 +584,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>24.385714285714283</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -605,7 +605,7 @@
         <v>31.000000000000004</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>42.285714285714285</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
         <v>1.5</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>23.914285714285711</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -647,7 +647,7 @@
         <v>1.6</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>20.457142857142856</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
         <v>28.8</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>29.685714285714287</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -689,7 +689,7 @@
         <v>23.4</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>24.342857142857145</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>24.400000000000002</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>20.228571428571428</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -752,7 +752,7 @@
         <v>0.3</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,7 +773,7 @@
         <v>8.4</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>21.157142857142855</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>74.899999999999991</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>24.11428571428571</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>33.1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>42.957142857142863</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -836,7 +836,7 @@
         <v>18.7</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>28.514285714285709</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -857,7 +857,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>26.900000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -878,7 +878,7 @@
         <v>21.900000000000002</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>26.428571428571427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
         <v>1.3</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>27.585714285714289</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>28.3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>28.028571428571432</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -941,7 +941,7 @@
         <v>20.200000000000003</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>34.928571428571431</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>57.6</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>32.199999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -983,7 +983,7 @@
         <v>23.2</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>36.328571428571429</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1004,7 +1004,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>24.599999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1025,7 +1025,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>20.471428571428568</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
         <v>11.9</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>31.714285714285715</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1067,7 +1067,7 @@
         <v>0.3</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>21.385714285714283</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
         <v>14</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>22.528571428571428</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1109,7 +1109,7 @@
         <v>13.3</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>22.071428571428573</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>18.3</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>16.099999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1151,7 +1151,7 @@
         <v>5.3999999999999995</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
         <v>38.5</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>21.842857142857145</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>5.7</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>21.828571428571426</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1214,7 +1214,7 @@
         <v>0.3</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>18.171428571428571</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1235,7 +1235,7 @@
         <v>0.3</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>26.657142857142855</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>40.199999999999996</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>15.857142857142856</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>